<commit_message>
feat: Merevisi struct Pasien penambahan Tanggal Lahir, revisi fungsi convert string to Date (menerima input format excel number)
</commit_message>
<xml_diff>
--- a/data/DataPMC20232024.xlsx
+++ b/data/DataPMC20232024.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Data Pasien"/>
@@ -1079,13 +1079,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1127,7 +1133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1150,35 +1156,44 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1484,33 +1499,33 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="20" width="19.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="7" width="19.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="7" width="13.43357142857143" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="19.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="16"/>
+      <c r="A1" s="18"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
       <c r="F1" s="9"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1541,7 @@
       <c r="E2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>157</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1539,20 +1554,20 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>163</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1568,20 +1583,20 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>168</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -1597,26 +1612,26 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>173</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="14">
         <v>49</v>
       </c>
       <c r="H5" s="4">
@@ -1626,26 +1641,26 @@
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="13" t="s">
         <v>178</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="14">
         <v>39</v>
       </c>
       <c r="H6" s="4">
@@ -1655,26 +1670,26 @@
         <v>180</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>184</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="14">
         <v>39</v>
       </c>
       <c r="H7" s="4">
@@ -1684,26 +1699,26 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>189</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="14">
         <v>39</v>
       </c>
       <c r="H8" s="4">
@@ -1713,26 +1728,26 @@
         <v>191</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>195</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="14">
         <v>46</v>
       </c>
       <c r="H9" s="4">
@@ -1742,26 +1757,26 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>199</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="14">
         <v>41</v>
       </c>
       <c r="H10" s="4">
@@ -1771,26 +1786,26 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>203</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="14">
         <v>38</v>
       </c>
       <c r="H11" s="4">
@@ -1800,26 +1815,26 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="13" t="s">
         <v>207</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="14">
         <v>44</v>
       </c>
       <c r="H12" s="4">
@@ -1829,26 +1844,26 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="19">
         <v>29857</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="14">
         <v>42</v>
       </c>
       <c r="H13" s="4">
@@ -1858,26 +1873,26 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="19">
         <v>28586</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="14">
         <v>46</v>
       </c>
       <c r="H14" s="4">
@@ -1887,26 +1902,26 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="13" t="s">
         <v>219</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="14">
         <v>46</v>
       </c>
       <c r="H15" s="4">
@@ -1916,26 +1931,26 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="13" t="s">
         <v>224</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="14">
         <v>41</v>
       </c>
       <c r="H16" s="4">
@@ -1952,19 +1967,19 @@
       <c r="B17" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="13" t="s">
         <v>224</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="14">
         <v>48</v>
       </c>
       <c r="H17" s="4">
@@ -1981,19 +1996,19 @@
       <c r="B18" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="19">
         <v>30570</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="14">
         <v>40</v>
       </c>
       <c r="H18" s="4">
@@ -2010,19 +2025,19 @@
       <c r="B19" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="13" t="s">
         <v>236</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="14">
         <v>47</v>
       </c>
       <c r="H19" s="4">
@@ -2039,19 +2054,19 @@
       <c r="B20" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="13" t="s">
         <v>194</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="14">
         <v>43</v>
       </c>
       <c r="H20" s="4">
@@ -2068,19 +2083,19 @@
       <c r="B21" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="13" t="s">
         <v>243</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="14">
         <v>47</v>
       </c>
       <c r="H21" s="4">
@@ -2097,19 +2112,19 @@
       <c r="B22" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="13" t="s">
         <v>195</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="14">
         <v>43</v>
       </c>
       <c r="H22" s="4">
@@ -2126,19 +2141,19 @@
       <c r="B23" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="19">
         <v>30427</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="14">
         <v>41</v>
       </c>
       <c r="H23" s="4">
@@ -2155,19 +2170,19 @@
       <c r="B24" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="13" t="s">
         <v>215</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="14">
         <v>49</v>
       </c>
       <c r="H24" s="4">
@@ -2184,19 +2199,19 @@
       <c r="B25" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="13" t="s">
         <v>173</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="14">
         <v>48</v>
       </c>
       <c r="H25" s="4">
@@ -2213,19 +2228,19 @@
       <c r="B26" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="13" t="s">
         <v>260</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="14">
         <v>40</v>
       </c>
       <c r="H26" s="4">
@@ -2242,19 +2257,19 @@
       <c r="B27" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="13" t="s">
         <v>264</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="14">
         <v>39</v>
       </c>
       <c r="H27" s="4">
@@ -2271,19 +2286,19 @@
       <c r="B28" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="13" t="s">
         <v>253</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="14">
         <v>38</v>
       </c>
       <c r="H28" s="4">
@@ -2300,19 +2315,19 @@
       <c r="B29" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="13" t="s">
         <v>189</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="14">
         <v>38</v>
       </c>
       <c r="H29" s="4">
@@ -2329,19 +2344,19 @@
       <c r="B30" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="19">
         <v>30575</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="14">
         <v>40</v>
       </c>
       <c r="H30" s="4">
@@ -2358,19 +2373,19 @@
       <c r="B31" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="F31" s="17">
+      <c r="F31" s="19">
         <v>28074</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="14">
         <v>47</v>
       </c>
       <c r="H31" s="4">
@@ -2387,19 +2402,19 @@
       <c r="B32" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="19">
         <v>29551</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="14">
         <v>43</v>
       </c>
       <c r="H32" s="4">
@@ -2416,19 +2431,19 @@
       <c r="B33" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="13" t="s">
         <v>283</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="14">
         <v>41</v>
       </c>
       <c r="H33" s="4">
@@ -2445,19 +2460,19 @@
       <c r="B34" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="19">
         <v>28004</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="14">
         <v>47</v>
       </c>
       <c r="H34" s="4">
@@ -2474,19 +2489,19 @@
       <c r="B35" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="13" t="s">
         <v>184</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="G35" s="13">
+      <c r="G35" s="14">
         <v>44</v>
       </c>
       <c r="H35" s="4">
@@ -2503,19 +2518,19 @@
       <c r="B36" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="13" t="s">
         <v>293</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="G36" s="13">
+      <c r="G36" s="14">
         <v>47</v>
       </c>
       <c r="H36" s="4">
@@ -2532,19 +2547,19 @@
       <c r="B37" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="13" t="s">
         <v>297</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="14">
         <v>43</v>
       </c>
       <c r="H37" s="4">
@@ -2561,19 +2576,19 @@
       <c r="B38" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="13" t="s">
         <v>303</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G38" s="14">
         <v>38</v>
       </c>
       <c r="H38" s="4">
@@ -2590,19 +2605,19 @@
       <c r="B39" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="13" t="s">
         <v>232</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="G39" s="13">
+      <c r="G39" s="14">
         <v>38</v>
       </c>
       <c r="H39" s="4">
@@ -2619,19 +2634,19 @@
       <c r="B40" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>310</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="G40" s="13">
+      <c r="G40" s="14">
         <v>46</v>
       </c>
       <c r="H40" s="4">
@@ -2648,19 +2663,19 @@
       <c r="B41" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F41" s="19">
         <v>29114</v>
       </c>
-      <c r="G41" s="13">
+      <c r="G41" s="14">
         <v>44</v>
       </c>
       <c r="H41" s="4">
@@ -2677,19 +2692,19 @@
       <c r="B42" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F42" s="19">
         <v>29856</v>
       </c>
-      <c r="G42" s="13">
+      <c r="G42" s="14">
         <v>42</v>
       </c>
       <c r="H42" s="4">
@@ -2706,19 +2721,19 @@
       <c r="B43" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="13" t="s">
         <v>253</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="14">
         <v>43</v>
       </c>
       <c r="H43" s="4">
@@ -2735,19 +2750,19 @@
       <c r="B44" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="13" t="s">
         <v>325</v>
       </c>
       <c r="F44" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="14">
         <v>43</v>
       </c>
       <c r="H44" s="4">
@@ -2764,19 +2779,19 @@
       <c r="B45" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="13" t="s">
         <v>329</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="14">
         <v>44</v>
       </c>
       <c r="H45" s="4">
@@ -2793,19 +2808,19 @@
       <c r="B46" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="F46" s="17">
+      <c r="F46" s="19">
         <v>30778</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="14">
         <v>40</v>
       </c>
       <c r="H46" s="4">
@@ -2822,19 +2837,19 @@
       <c r="B47" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="13" t="s">
         <v>335</v>
       </c>
       <c r="F47" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="G47" s="13">
+      <c r="G47" s="14">
         <v>44</v>
       </c>
       <c r="H47" s="4">
@@ -2851,19 +2866,19 @@
       <c r="B48" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="F48" s="17">
+      <c r="F48" s="19">
         <v>29335</v>
       </c>
-      <c r="G48" s="13">
+      <c r="G48" s="14">
         <v>44</v>
       </c>
       <c r="H48" s="4">
@@ -2880,19 +2895,19 @@
       <c r="B49" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="13" t="s">
         <v>243</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="14">
         <v>43</v>
       </c>
       <c r="H49" s="4">
@@ -2909,19 +2924,19 @@
       <c r="B50" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="13" t="s">
         <v>325</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="14">
         <v>43</v>
       </c>
       <c r="H50" s="4">
@@ -2938,19 +2953,19 @@
       <c r="B51" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="13" t="s">
         <v>345</v>
       </c>
       <c r="F51" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="14">
         <v>40</v>
       </c>
       <c r="H51" s="4">
@@ -2967,19 +2982,19 @@
       <c r="B52" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="13" t="s">
         <v>303</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="G52" s="13">
+      <c r="G52" s="14">
         <v>41</v>
       </c>
       <c r="H52" s="4">
@@ -3006,20 +3021,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="22.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="22.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="19.290714285714284" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="8"/>
       <c r="B1" s="9"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
       <c r="F1" s="9"/>
       <c r="G1" s="8"/>
     </row>
@@ -3027,7 +3042,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -3039,7 +3054,7 @@
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -3053,13 +3068,13 @@
       <c r="B3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -3073,22 +3088,22 @@
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3096,22 +3111,22 @@
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="15">
         <v>45172</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="15">
         <v>45175</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3119,22 +3134,22 @@
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="15">
         <v>45231</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="15">
         <v>45234</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3142,22 +3157,22 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3165,22 +3180,22 @@
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="15">
         <v>44814</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="15">
         <v>44817</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3188,22 +3203,22 @@
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3211,22 +3226,22 @@
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3234,22 +3249,22 @@
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3257,22 +3272,22 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -3280,22 +3295,22 @@
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="15">
         <v>44661</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="15">
         <v>44664</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -3303,22 +3318,22 @@
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="15">
         <v>44671</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="15">
         <v>44674</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3326,22 +3341,22 @@
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3349,22 +3364,22 @@
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="15">
         <v>45025</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="15">
         <v>45028</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3372,22 +3387,22 @@
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3395,22 +3410,22 @@
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -3418,22 +3433,22 @@
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3441,22 +3456,22 @@
       <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3464,22 +3479,22 @@
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="15">
         <v>44831</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="15">
         <v>44834</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3487,22 +3502,22 @@
       <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3510,22 +3525,22 @@
       <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="15">
         <v>45172</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="15">
         <v>45175</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3533,22 +3548,22 @@
       <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -3556,22 +3571,22 @@
       <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3579,22 +3594,22 @@
       <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3602,22 +3617,22 @@
       <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3625,22 +3640,22 @@
       <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3648,22 +3663,22 @@
       <c r="A29" s="4">
         <v>27</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="15">
         <v>44678</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="15">
         <v>44681</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3671,22 +3686,22 @@
       <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="15">
         <v>45172</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="15">
         <v>45175</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3694,22 +3709,22 @@
       <c r="A31" s="4">
         <v>29</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3717,22 +3732,22 @@
       <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="15">
         <v>45172</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="15">
         <v>45175</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3740,22 +3755,22 @@
       <c r="A33" s="4">
         <v>31</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="15">
         <v>45023</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="15">
         <v>45026</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -3763,22 +3778,22 @@
       <c r="A34" s="4">
         <v>32</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -3786,22 +3801,22 @@
       <c r="A35" s="4">
         <v>33</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="15">
         <v>45196</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="15">
         <v>45199</v>
       </c>
-      <c r="G35" s="13">
+      <c r="G35" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3809,22 +3824,22 @@
       <c r="A36" s="4">
         <v>34</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G36" s="13">
+      <c r="G36" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3832,22 +3847,22 @@
       <c r="A37" s="4">
         <v>35</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -3855,22 +3870,22 @@
       <c r="A38" s="4">
         <v>36</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="15">
         <v>45181</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="14">
+      <c r="F38" s="15">
         <v>45184</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G38" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3878,22 +3893,22 @@
       <c r="A39" s="4">
         <v>37</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G39" s="13">
+      <c r="G39" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -3901,22 +3916,22 @@
       <c r="A40" s="4">
         <v>38</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G40" s="13">
+      <c r="G40" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -3924,22 +3939,22 @@
       <c r="A41" s="4">
         <v>39</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="G41" s="13">
+      <c r="G41" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -3947,22 +3962,22 @@
       <c r="A42" s="4">
         <v>40</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G42" s="13">
+      <c r="G42" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -3970,22 +3985,22 @@
       <c r="A43" s="4">
         <v>41</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -3993,22 +4008,22 @@
       <c r="A44" s="4">
         <v>42</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -4016,22 +4031,22 @@
       <c r="A45" s="4">
         <v>43</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4039,22 +4054,22 @@
       <c r="A46" s="4">
         <v>44</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4062,22 +4077,22 @@
       <c r="A47" s="4">
         <v>45</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F47" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G47" s="13">
+      <c r="G47" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -4085,22 +4100,22 @@
       <c r="A48" s="4">
         <v>46</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G48" s="13">
+      <c r="G48" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -4108,22 +4123,22 @@
       <c r="A49" s="4">
         <v>47</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -4131,22 +4146,22 @@
       <c r="A50" s="4">
         <v>48</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F50" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4154,22 +4169,22 @@
       <c r="A51" s="4">
         <v>49</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -4177,22 +4192,22 @@
       <c r="A52" s="4">
         <v>50</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="G52" s="13">
+      <c r="G52" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -4200,22 +4215,22 @@
       <c r="A53" s="4">
         <v>51</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F53" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="13">
+      <c r="G53" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -4223,22 +4238,22 @@
       <c r="A54" s="4">
         <v>52</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F54" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G54" s="13">
+      <c r="G54" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -4246,22 +4261,22 @@
       <c r="A55" s="4">
         <v>53</v>
       </c>
-      <c r="B55" s="14">
+      <c r="B55" s="15">
         <v>45194</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="14">
+      <c r="F55" s="15">
         <v>45197</v>
       </c>
-      <c r="G55" s="13">
+      <c r="G55" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4269,22 +4284,22 @@
       <c r="A56" s="4">
         <v>54</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="11" t="s">
+      <c r="F56" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="G56" s="13">
+      <c r="G56" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -4292,22 +4307,22 @@
       <c r="A57" s="4">
         <v>55</v>
       </c>
-      <c r="B57" s="14">
+      <c r="B57" s="15">
         <v>44823</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="14">
+      <c r="F57" s="15">
         <v>44826</v>
       </c>
-      <c r="G57" s="13">
+      <c r="G57" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4315,22 +4330,22 @@
       <c r="A58" s="4">
         <v>56</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="F58" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G58" s="13">
+      <c r="G58" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -4338,22 +4353,22 @@
       <c r="A59" s="4">
         <v>57</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="12" t="s">
+      <c r="E59" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="G59" s="13">
+      <c r="G59" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -4361,22 +4376,22 @@
       <c r="A60" s="4">
         <v>58</v>
       </c>
-      <c r="B60" s="14">
+      <c r="B60" s="15">
         <v>44876</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="D60" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E60" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="14">
+      <c r="F60" s="15">
         <v>44879</v>
       </c>
-      <c r="G60" s="13">
+      <c r="G60" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4384,22 +4399,22 @@
       <c r="A61" s="4">
         <v>59</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F61" s="11" t="s">
+      <c r="F61" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G61" s="13">
+      <c r="G61" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -4407,22 +4422,22 @@
       <c r="A62" s="4">
         <v>60</v>
       </c>
-      <c r="B62" s="14">
+      <c r="B62" s="15">
         <v>44813</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="D62" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E62" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="14">
+      <c r="F62" s="15">
         <v>44816</v>
       </c>
-      <c r="G62" s="13">
+      <c r="G62" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -4430,22 +4445,22 @@
       <c r="A63" s="4">
         <v>61</v>
       </c>
-      <c r="B63" s="14">
+      <c r="B63" s="15">
         <v>45175</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D63" s="12" t="s">
+      <c r="D63" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="14">
+      <c r="F63" s="15">
         <v>45178</v>
       </c>
-      <c r="G63" s="13">
+      <c r="G63" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4453,22 +4468,22 @@
       <c r="A64" s="4">
         <v>62</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D64" s="12" t="s">
+      <c r="D64" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="11" t="s">
+      <c r="F64" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G64" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4476,22 +4491,22 @@
       <c r="A65" s="4">
         <v>63</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="12" t="s">
+      <c r="C65" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="12" t="s">
+      <c r="D65" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="11" t="s">
+      <c r="F65" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="G65" s="13">
+      <c r="G65" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4499,22 +4514,22 @@
       <c r="A66" s="4">
         <v>64</v>
       </c>
-      <c r="B66" s="14">
+      <c r="B66" s="15">
         <v>45180</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F66" s="14">
+      <c r="F66" s="15">
         <v>45183</v>
       </c>
-      <c r="G66" s="13">
+      <c r="G66" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -4522,22 +4537,22 @@
       <c r="A67" s="4">
         <v>65</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="12" t="s">
+      <c r="C67" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E67" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F67" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="G67" s="13">
+      <c r="G67" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -4545,22 +4560,22 @@
       <c r="A68" s="4">
         <v>66</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="12" t="s">
+      <c r="C68" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F68" s="11" t="s">
+      <c r="F68" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="G68" s="13">
+      <c r="G68" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4568,22 +4583,22 @@
       <c r="A69" s="4">
         <v>67</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="12" t="s">
+      <c r="C69" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D69" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F69" s="11" t="s">
+      <c r="F69" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G69" s="13">
+      <c r="G69" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -4591,22 +4606,22 @@
       <c r="A70" s="4">
         <v>68</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C70" s="12" t="s">
+      <c r="C70" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="D70" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E70" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F70" s="11" t="s">
+      <c r="F70" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="G70" s="13">
+      <c r="G70" s="14">
         <v>265000</v>
       </c>
     </row>
@@ -4614,22 +4629,22 @@
       <c r="A71" s="4">
         <v>69</v>
       </c>
-      <c r="B71" s="14">
+      <c r="B71" s="15">
         <v>45035</v>
       </c>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D71" s="12" t="s">
+      <c r="D71" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E71" s="12" t="s">
+      <c r="E71" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F71" s="14">
+      <c r="F71" s="15">
         <v>45038</v>
       </c>
-      <c r="G71" s="13">
+      <c r="G71" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4637,22 +4652,22 @@
       <c r="A72" s="4">
         <v>70</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C72" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="D72" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E72" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F72" s="11" t="s">
+      <c r="F72" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="G72" s="13">
+      <c r="G72" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -4660,22 +4675,22 @@
       <c r="A73" s="4">
         <v>71</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="12" t="s">
+      <c r="C73" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D73" s="12" t="s">
+      <c r="D73" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F73" s="11" t="s">
+      <c r="F73" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="G73" s="13">
+      <c r="G73" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4683,22 +4698,22 @@
       <c r="A74" s="4">
         <v>72</v>
       </c>
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C74" s="12" t="s">
+      <c r="C74" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D74" s="12" t="s">
+      <c r="D74" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="E74" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="F74" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="G74" s="13">
+      <c r="G74" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4706,22 +4721,22 @@
       <c r="A75" s="4">
         <v>73</v>
       </c>
-      <c r="B75" s="14">
+      <c r="B75" s="15">
         <v>45034</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C75" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D75" s="12" t="s">
+      <c r="D75" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F75" s="14">
+      <c r="F75" s="15">
         <v>45037</v>
       </c>
-      <c r="G75" s="13">
+      <c r="G75" s="14">
         <v>290000</v>
       </c>
     </row>
@@ -4729,22 +4744,22 @@
       <c r="A76" s="4">
         <v>74</v>
       </c>
-      <c r="B76" s="14">
+      <c r="B76" s="15">
         <v>44661</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C76" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D76" s="12" t="s">
+      <c r="D76" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E76" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="14">
+      <c r="F76" s="15">
         <v>44664</v>
       </c>
-      <c r="G76" s="13">
+      <c r="G76" s="14">
         <v>240000</v>
       </c>
     </row>
@@ -4752,22 +4767,22 @@
       <c r="A77" s="4">
         <v>75</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D77" s="12" t="s">
+      <c r="D77" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F77" s="11" t="s">
+      <c r="F77" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="G77" s="13">
+      <c r="G77" s="14">
         <v>165000</v>
       </c>
     </row>
@@ -4783,7 +4798,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
git commit -m "Update dataOperator.c dengan fungsi createIDPatient()"
</commit_message>
<xml_diff>
--- a/data/DataPMC20232024.xlsx
+++ b/data/DataPMC20232024.xlsx
@@ -1133,7 +1133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1156,13 +1156,10 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -1186,14 +1183,8 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1505,24 +1496,24 @@
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="20" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="15" width="19.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="7" width="19.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="7" width="13.43357142857143" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="19.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="18"/>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
       <c r="I1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
@@ -1541,7 +1532,7 @@
       <c r="E2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>157</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1554,23 +1545,23 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>164</v>
       </c>
       <c r="G3" s="4">
@@ -1583,23 +1574,23 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>169</v>
       </c>
       <c r="G4" s="4">
@@ -1609,29 +1600,29 @@
         <v>1234567891</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>49</v>
       </c>
       <c r="H5" s="4">
@@ -1641,26 +1632,26 @@
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>39</v>
       </c>
       <c r="H6" s="4">
@@ -1670,26 +1661,26 @@
         <v>180</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>39</v>
       </c>
       <c r="H7" s="4">
@@ -1699,26 +1690,26 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>39</v>
       </c>
       <c r="H8" s="4">
@@ -1728,26 +1719,26 @@
         <v>191</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <v>46</v>
       </c>
       <c r="H9" s="4">
@@ -1757,26 +1748,26 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>41</v>
       </c>
       <c r="H10" s="4">
@@ -1786,26 +1777,26 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>38</v>
       </c>
       <c r="H11" s="4">
@@ -1815,26 +1806,26 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>44</v>
       </c>
       <c r="H12" s="4">
@@ -1844,26 +1835,26 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="17">
         <v>29857</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <v>42</v>
       </c>
       <c r="H13" s="4">
@@ -1873,26 +1864,26 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="17">
         <v>28586</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <v>46</v>
       </c>
       <c r="H14" s="4">
@@ -1909,19 +1900,19 @@
       <c r="B15" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="13">
         <v>46</v>
       </c>
       <c r="H15" s="4">
@@ -1938,19 +1929,19 @@
       <c r="B16" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <v>41</v>
       </c>
       <c r="H16" s="4">
@@ -1967,19 +1958,19 @@
       <c r="B17" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <v>48</v>
       </c>
       <c r="H17" s="4">
@@ -1996,19 +1987,19 @@
       <c r="B18" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="17">
         <v>30570</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>40</v>
       </c>
       <c r="H18" s="4">
@@ -2025,19 +2016,19 @@
       <c r="B19" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>47</v>
       </c>
       <c r="H19" s="4">
@@ -2054,19 +2045,19 @@
       <c r="B20" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <v>43</v>
       </c>
       <c r="H20" s="4">
@@ -2083,19 +2074,19 @@
       <c r="B21" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>47</v>
       </c>
       <c r="H21" s="4">
@@ -2112,19 +2103,19 @@
       <c r="B22" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <v>43</v>
       </c>
       <c r="H22" s="4">
@@ -2141,19 +2132,19 @@
       <c r="B23" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="17">
         <v>30427</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <v>41</v>
       </c>
       <c r="H23" s="4">
@@ -2170,19 +2161,19 @@
       <c r="B24" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <v>49</v>
       </c>
       <c r="H24" s="4">
@@ -2199,19 +2190,19 @@
       <c r="B25" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <v>48</v>
       </c>
       <c r="H25" s="4">
@@ -2228,19 +2219,19 @@
       <c r="B26" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <v>40</v>
       </c>
       <c r="H26" s="4">
@@ -2257,19 +2248,19 @@
       <c r="B27" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <v>39</v>
       </c>
       <c r="H27" s="4">
@@ -2286,19 +2277,19 @@
       <c r="B28" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <v>38</v>
       </c>
       <c r="H28" s="4">
@@ -2315,19 +2306,19 @@
       <c r="B29" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="13">
         <v>38</v>
       </c>
       <c r="H29" s="4">
@@ -2344,19 +2335,19 @@
       <c r="B30" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="17">
         <v>30575</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="13">
         <v>40</v>
       </c>
       <c r="H30" s="4">
@@ -2373,19 +2364,19 @@
       <c r="B31" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="17">
         <v>28074</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <v>47</v>
       </c>
       <c r="H31" s="4">
@@ -2402,19 +2393,19 @@
       <c r="B32" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F32" s="17">
         <v>29551</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <v>43</v>
       </c>
       <c r="H32" s="4">
@@ -2431,19 +2422,19 @@
       <c r="B33" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <v>41</v>
       </c>
       <c r="H33" s="4">
@@ -2460,19 +2451,19 @@
       <c r="B34" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="17">
         <v>28004</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="13">
         <v>47</v>
       </c>
       <c r="H34" s="4">
@@ -2489,19 +2480,19 @@
       <c r="B35" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <v>44</v>
       </c>
       <c r="H35" s="4">
@@ -2518,19 +2509,19 @@
       <c r="B36" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <v>47</v>
       </c>
       <c r="H36" s="4">
@@ -2547,19 +2538,19 @@
       <c r="B37" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E37" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="13">
         <v>43</v>
       </c>
       <c r="H37" s="4">
@@ -2576,19 +2567,19 @@
       <c r="B38" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="13">
         <v>38</v>
       </c>
       <c r="H38" s="4">
@@ -2605,19 +2596,19 @@
       <c r="B39" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="13">
         <v>38</v>
       </c>
       <c r="H39" s="4">
@@ -2634,19 +2625,19 @@
       <c r="B40" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E40" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="13">
         <v>46</v>
       </c>
       <c r="H40" s="4">
@@ -2663,19 +2654,19 @@
       <c r="B41" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="F41" s="19">
+      <c r="F41" s="17">
         <v>29114</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="13">
         <v>44</v>
       </c>
       <c r="H41" s="4">
@@ -2692,19 +2683,19 @@
       <c r="B42" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E42" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F42" s="17">
         <v>29856</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="13">
         <v>42</v>
       </c>
       <c r="H42" s="4">
@@ -2721,19 +2712,19 @@
       <c r="B43" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E43" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="13">
         <v>43</v>
       </c>
       <c r="H43" s="4">
@@ -2750,19 +2741,19 @@
       <c r="B44" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E44" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G44" s="13">
         <v>43</v>
       </c>
       <c r="H44" s="4">
@@ -2779,19 +2770,19 @@
       <c r="B45" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="13">
         <v>44</v>
       </c>
       <c r="H45" s="4">
@@ -2808,19 +2799,19 @@
       <c r="B46" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E46" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="F46" s="19">
+      <c r="F46" s="17">
         <v>30778</v>
       </c>
-      <c r="G46" s="14">
+      <c r="G46" s="13">
         <v>40</v>
       </c>
       <c r="H46" s="4">
@@ -2837,19 +2828,19 @@
       <c r="B47" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>334</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="12" t="s">
         <v>335</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="13">
         <v>44</v>
       </c>
       <c r="H47" s="4">
@@ -2866,19 +2857,19 @@
       <c r="B48" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E48" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="F48" s="19">
+      <c r="F48" s="17">
         <v>29335</v>
       </c>
-      <c r="G48" s="14">
+      <c r="G48" s="13">
         <v>44</v>
       </c>
       <c r="H48" s="4">
@@ -2895,19 +2886,19 @@
       <c r="B49" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G49" s="13">
         <v>43</v>
       </c>
       <c r="H49" s="4">
@@ -2924,19 +2915,19 @@
       <c r="B50" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="E50" s="13" t="s">
+      <c r="E50" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="G50" s="14">
+      <c r="G50" s="13">
         <v>43</v>
       </c>
       <c r="H50" s="4">
@@ -2953,19 +2944,19 @@
       <c r="B51" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="G51" s="14">
+      <c r="G51" s="13">
         <v>40</v>
       </c>
       <c r="H51" s="4">
@@ -2982,19 +2973,19 @@
       <c r="B52" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D52" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E52" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="G52" s="14">
+      <c r="G52" s="13">
         <v>41</v>
       </c>
       <c r="H52" s="4">
@@ -3021,28 +3012,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="22.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="22.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="15" width="19.290714285714284" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="8"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -3054,7 +3045,7 @@
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -3065,19 +3056,19 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="4">
@@ -3088,22 +3079,22 @@
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3111,22 +3102,22 @@
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>45172</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>45175</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3134,22 +3125,22 @@
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>45231</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>45234</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3157,22 +3148,22 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3180,22 +3171,22 @@
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>44814</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>44817</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3203,22 +3194,22 @@
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3226,22 +3217,22 @@
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3249,22 +3240,22 @@
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3272,22 +3263,22 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -3295,22 +3286,22 @@
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>44661</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <v>44664</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -3318,22 +3309,22 @@
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>44671</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <v>44674</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3341,22 +3332,22 @@
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3364,22 +3355,22 @@
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>45025</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <v>45028</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3387,22 +3378,22 @@
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3410,22 +3401,22 @@
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -3433,22 +3424,22 @@
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3456,22 +3447,22 @@
       <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3479,22 +3470,22 @@
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>44831</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="14">
         <v>44834</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3502,22 +3493,22 @@
       <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3525,22 +3516,22 @@
       <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="14">
         <v>45172</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="14">
         <v>45175</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3548,22 +3539,22 @@
       <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -3571,22 +3562,22 @@
       <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3594,22 +3585,22 @@
       <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3617,22 +3608,22 @@
       <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3640,22 +3631,22 @@
       <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3663,22 +3654,22 @@
       <c r="A29" s="4">
         <v>27</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>44678</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="14">
         <v>44681</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3686,22 +3677,22 @@
       <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>45172</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="14">
         <v>45175</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3709,22 +3700,22 @@
       <c r="A31" s="4">
         <v>29</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3732,22 +3723,22 @@
       <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="14">
         <v>45172</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="14">
         <v>45175</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3755,22 +3746,22 @@
       <c r="A33" s="4">
         <v>31</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="14">
         <v>45023</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="14">
         <v>45026</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -3778,22 +3769,22 @@
       <c r="A34" s="4">
         <v>32</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -3801,22 +3792,22 @@
       <c r="A35" s="4">
         <v>33</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="14">
         <v>45196</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="14">
         <v>45199</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3824,22 +3815,22 @@
       <c r="A36" s="4">
         <v>34</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3847,22 +3838,22 @@
       <c r="A37" s="4">
         <v>35</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E37" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -3870,22 +3861,22 @@
       <c r="A38" s="4">
         <v>36</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="14">
         <v>45181</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="14">
         <v>45184</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3893,22 +3884,22 @@
       <c r="A39" s="4">
         <v>37</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -3916,22 +3907,22 @@
       <c r="A40" s="4">
         <v>38</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E40" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -3939,22 +3930,22 @@
       <c r="A41" s="4">
         <v>39</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -3962,22 +3953,22 @@
       <c r="A42" s="4">
         <v>40</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E42" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -3985,22 +3976,22 @@
       <c r="A43" s="4">
         <v>41</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E43" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4008,22 +3999,22 @@
       <c r="A44" s="4">
         <v>42</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E44" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G44" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -4031,22 +4022,22 @@
       <c r="A45" s="4">
         <v>43</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4054,22 +4045,22 @@
       <c r="A46" s="4">
         <v>44</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E46" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="14">
+      <c r="G46" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4077,22 +4068,22 @@
       <c r="A47" s="4">
         <v>45</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -4100,22 +4091,22 @@
       <c r="A48" s="4">
         <v>46</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E48" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G48" s="14">
+      <c r="G48" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -4123,22 +4114,22 @@
       <c r="A49" s="4">
         <v>47</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G49" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4146,22 +4137,22 @@
       <c r="A50" s="4">
         <v>48</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="13" t="s">
+      <c r="E50" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G50" s="14">
+      <c r="G50" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4169,22 +4160,22 @@
       <c r="A51" s="4">
         <v>49</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F51" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="G51" s="14">
+      <c r="G51" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4192,22 +4183,22 @@
       <c r="A52" s="4">
         <v>50</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D52" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E52" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="G52" s="14">
+      <c r="G52" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4215,22 +4206,22 @@
       <c r="A53" s="4">
         <v>51</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="14">
+      <c r="G53" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -4238,22 +4229,22 @@
       <c r="A54" s="4">
         <v>52</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D54" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E54" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="G54" s="14">
+      <c r="G54" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -4261,22 +4252,22 @@
       <c r="A55" s="4">
         <v>53</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="14">
         <v>45194</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="15">
+      <c r="F55" s="14">
         <v>45197</v>
       </c>
-      <c r="G55" s="14">
+      <c r="G55" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4284,22 +4275,22 @@
       <c r="A56" s="4">
         <v>54</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D56" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E56" s="13" t="s">
+      <c r="E56" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="G56" s="14">
+      <c r="G56" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -4307,22 +4298,22 @@
       <c r="A57" s="4">
         <v>55</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="14">
         <v>44823</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E57" s="13" t="s">
+      <c r="E57" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="15">
+      <c r="F57" s="14">
         <v>44826</v>
       </c>
-      <c r="G57" s="14">
+      <c r="G57" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4330,22 +4321,22 @@
       <c r="A58" s="4">
         <v>56</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="G58" s="14">
+      <c r="G58" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4353,22 +4344,22 @@
       <c r="A59" s="4">
         <v>57</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B59" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="13" t="s">
+      <c r="E59" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F59" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="G59" s="14">
+      <c r="G59" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4376,22 +4367,22 @@
       <c r="A60" s="4">
         <v>58</v>
       </c>
-      <c r="B60" s="15">
+      <c r="B60" s="14">
         <v>44876</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="D60" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="13" t="s">
+      <c r="E60" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="15">
+      <c r="F60" s="14">
         <v>44879</v>
       </c>
-      <c r="G60" s="14">
+      <c r="G60" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4399,22 +4390,22 @@
       <c r="A61" s="4">
         <v>59</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D61" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E61" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F61" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="G61" s="14">
+      <c r="G61" s="13">
         <v>165000</v>
       </c>
     </row>
@@ -4422,22 +4413,22 @@
       <c r="A62" s="4">
         <v>60</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="14">
         <v>44813</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E62" s="13" t="s">
+      <c r="E62" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="15">
+      <c r="F62" s="14">
         <v>44816</v>
       </c>
-      <c r="G62" s="14">
+      <c r="G62" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -4445,22 +4436,22 @@
       <c r="A63" s="4">
         <v>61</v>
       </c>
-      <c r="B63" s="15">
+      <c r="B63" s="14">
         <v>45175</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D63" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E63" s="13" t="s">
+      <c r="E63" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="15">
+      <c r="F63" s="14">
         <v>45178</v>
       </c>
-      <c r="G63" s="14">
+      <c r="G63" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4468,22 +4459,22 @@
       <c r="A64" s="4">
         <v>62</v>
       </c>
-      <c r="B64" s="12" t="s">
+      <c r="B64" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="D64" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E64" s="13" t="s">
+      <c r="E64" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="12" t="s">
+      <c r="F64" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="G64" s="14">
+      <c r="G64" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4491,22 +4482,22 @@
       <c r="A65" s="4">
         <v>63</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C65" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D65" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E65" s="13" t="s">
+      <c r="E65" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="F65" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="G65" s="14">
+      <c r="G65" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4514,22 +4505,22 @@
       <c r="A66" s="4">
         <v>64</v>
       </c>
-      <c r="B66" s="15">
+      <c r="B66" s="14">
         <v>45180</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="D66" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E66" s="13" t="s">
+      <c r="E66" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F66" s="15">
+      <c r="F66" s="14">
         <v>45183</v>
       </c>
-      <c r="G66" s="14">
+      <c r="G66" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4537,22 +4528,22 @@
       <c r="A67" s="4">
         <v>65</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C67" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D67" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E67" s="13" t="s">
+      <c r="E67" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="F67" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="G67" s="14">
+      <c r="G67" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -4560,22 +4551,22 @@
       <c r="A68" s="4">
         <v>66</v>
       </c>
-      <c r="B68" s="12" t="s">
+      <c r="B68" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="13" t="s">
+      <c r="C68" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D68" s="13" t="s">
+      <c r="D68" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E68" s="13" t="s">
+      <c r="E68" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F68" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="G68" s="14">
+      <c r="G68" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4583,22 +4574,22 @@
       <c r="A69" s="4">
         <v>67</v>
       </c>
-      <c r="B69" s="12" t="s">
+      <c r="B69" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="D69" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E69" s="13" t="s">
+      <c r="E69" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="G69" s="14">
+      <c r="G69" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4606,22 +4597,22 @@
       <c r="A70" s="4">
         <v>68</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B70" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C70" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D70" s="13" t="s">
+      <c r="D70" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="13" t="s">
+      <c r="E70" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="G70" s="14">
+      <c r="G70" s="13">
         <v>265000</v>
       </c>
     </row>
@@ -4629,22 +4620,22 @@
       <c r="A71" s="4">
         <v>69</v>
       </c>
-      <c r="B71" s="15">
+      <c r="B71" s="14">
         <v>45035</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E71" s="13" t="s">
+      <c r="E71" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F71" s="15">
+      <c r="F71" s="14">
         <v>45038</v>
       </c>
-      <c r="G71" s="14">
+      <c r="G71" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4652,22 +4643,22 @@
       <c r="A72" s="4">
         <v>70</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="D72" s="13" t="s">
+      <c r="D72" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E72" s="13" t="s">
+      <c r="E72" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="G72" s="14">
+      <c r="G72" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4675,22 +4666,22 @@
       <c r="A73" s="4">
         <v>71</v>
       </c>
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="D73" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="13" t="s">
+      <c r="E73" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G73" s="14">
+      <c r="G73" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4698,22 +4689,22 @@
       <c r="A74" s="4">
         <v>72</v>
       </c>
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D74" s="13" t="s">
+      <c r="D74" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E74" s="13" t="s">
+      <c r="E74" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F74" s="12" t="s">
+      <c r="F74" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="G74" s="14">
+      <c r="G74" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4721,22 +4712,22 @@
       <c r="A75" s="4">
         <v>73</v>
       </c>
-      <c r="B75" s="15">
+      <c r="B75" s="14">
         <v>45034</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D75" s="13" t="s">
+      <c r="D75" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E75" s="13" t="s">
+      <c r="E75" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F75" s="15">
+      <c r="F75" s="14">
         <v>45037</v>
       </c>
-      <c r="G75" s="14">
+      <c r="G75" s="13">
         <v>290000</v>
       </c>
     </row>
@@ -4744,22 +4735,22 @@
       <c r="A76" s="4">
         <v>74</v>
       </c>
-      <c r="B76" s="15">
+      <c r="B76" s="14">
         <v>44661</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D76" s="13" t="s">
+      <c r="D76" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E76" s="13" t="s">
+      <c r="E76" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="15">
+      <c r="F76" s="14">
         <v>44664</v>
       </c>
-      <c r="G76" s="14">
+      <c r="G76" s="13">
         <v>240000</v>
       </c>
     </row>
@@ -4767,22 +4758,22 @@
       <c r="A77" s="4">
         <v>75</v>
       </c>
-      <c r="B77" s="12" t="s">
+      <c r="B77" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D77" s="13" t="s">
+      <c r="D77" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E77" s="13" t="s">
+      <c r="E77" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="G77" s="14">
+      <c r="G77" s="13">
         <v>165000</v>
       </c>
     </row>

</xml_diff>